<commit_message>
atualização do mapa mental
</commit_message>
<xml_diff>
--- a/Planilhas/dados_PETR4_2024.09.17.xlsx
+++ b/Planilhas/dados_PETR4_2024.09.17.xlsx
@@ -7,7 +7,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BBC712-7BED-42ED-BF41-9128B83F1EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C47AD7-CF98-444D-AE1F-331C48F1A03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
@@ -1437,12 +1437,6 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.00"/>
-      <color rgb="FF000000"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.00"/>
       <u val="single"/>
       <color rgb="FF0000FF"/>
       <family val="2"/>
@@ -1451,6 +1445,12 @@
       <name val="Calibri"/>
       <sz val="11.00"/>
       <b/>
+      <color rgb="FF000000"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.00"/>
       <color rgb="FF000000"/>
       <family val="2"/>
     </font>
@@ -1490,18 +1490,18 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf fontId="1" applyFont="1"/>
-    <xf fontId="2" applyFont="1"/>
-    <xf fontId="3" applyFont="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" applyFont="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" horizontal="center"/>
     </xf>
+    <xf fontId="3" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf xfId="3" quotePrefix="0" pivotButton="0" fontId="3" applyFont="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="2" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" horizontal="center"/>
     </xf>
+    <xf xfId="3" quotePrefix="0" pivotButton="0" fontId="3" applyFont="1"/>
     <xf xfId="1" quotePrefix="0" pivotButton="0" fontId="1" applyFont="1"/>
-    <xf xfId="2" quotePrefix="0" pivotButton="0" fontId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normal" xfId="0" builtinId="0"/>
@@ -6682,7 +6682,7 @@
         <v>717735583740</v>
       </c>
       <c r="BW3" s="2">
-        <v>23.9747999999998</v>
+        <v>23.9747999999997</v>
       </c>
       <c r="BX3" s="2">
         <v>2.3119</v>
@@ -59145,7 +59145,7 @@
         <v>36.99</v>
       </c>
       <c r="Y2" s="2">
-        <v>37.0499999999998</v>
+        <v>37.0499999999997</v>
       </c>
       <c r="Z2" s="2">
         <v>0</v>
@@ -59160,7 +59160,7 @@
         <v>0</v>
       </c>
       <c r="AD2" s="2">
-        <v>42.9399999999998</v>
+        <v>42.9399999999997</v>
       </c>
       <c r="AE2" s="2">
         <v>1.0094349</v>
@@ -59339,7 +59339,7 @@
         <v>499064995840</v>
       </c>
       <c r="Q2" s="2">
-        <v>88.1479999999998</v>
+        <v>88.1479999999997</v>
       </c>
       <c r="R2" s="2">
         <v>38.524</v>
@@ -60024,7 +60024,7 @@
         <v>214</v>
       </c>
       <c r="R2" s="2">
-        <v>87.7399999999998</v>
+        <v>87.7399999999997</v>
       </c>
       <c r="V2" s="2" t="b">
         <v>0</v>

</xml_diff>